<commit_message>
Rewrote unittest to properly look for test bank for test workbooks
</commit_message>
<xml_diff>
--- a/test_spreadsheets/2-Cleaning Samples Template.xlsx
+++ b/test_spreadsheets/2-Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">Sample Set:</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Stainless Steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test if program exits with type error</t>
   </si>
   <si>
     <t xml:space="preserve">Result Set ID:</t>
@@ -437,7 +440,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -472,19 +475,19 @@
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>1.25</v>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>20</v>
@@ -492,13 +495,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>1.16</v>
@@ -506,13 +509,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>1.1</v>
@@ -520,7 +523,7 @@
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>20</v>
@@ -530,7 +533,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>20</v>
@@ -540,29 +543,29 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -572,40 +575,40 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,17 +616,17 @@
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,13 +634,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>10</v>
@@ -649,13 +652,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0.024</v>
@@ -669,13 +672,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0.35</v>
@@ -689,13 +692,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>0.14</v>

</xml_diff>